<commit_message>
Se modifican las fechas de entrega de los Sprints
</commit_message>
<xml_diff>
--- a/Documentacion/Product_Backlog-ParkingApp.xlsx
+++ b/Documentacion/Product_Backlog-ParkingApp.xlsx
@@ -153,7 +153,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="51">
   <si>
     <t>Increment Plan</t>
   </si>
@@ -303,6 +303,9 @@
   </si>
   <si>
     <t>Creación de modulo para generación de factura</t>
+  </si>
+  <si>
+    <t>7/22/2021</t>
   </si>
 </sst>
 </file>
@@ -681,37 +684,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Porcentaje" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="41">
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="54"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="54"/>
-      </font>
-    </dxf>
+  <dxfs count="37">
     <dxf>
       <fill>
         <patternFill patternType="lightUp">
@@ -1503,7 +1476,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1515,7 +1488,7 @@
   <dimension ref="A1:K32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2270,15 +2243,15 @@
       </c>
       <c r="B4" s="8">
         <f>IF(OR(B16="",A4=""),"",B16)</f>
-        <v>44448</v>
+        <v>44501</v>
       </c>
       <c r="C4" s="7">
         <f t="shared" ref="C4:C10" si="0">IF(A4="","",SUMIF(J$16:J$30,A4,C$16:C$30))</f>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D4" s="8">
         <f t="shared" ref="D4:D10" si="1">IF(OR(B4="",C4=""),"",B4+C4-1)</f>
-        <v>44455</v>
+        <v>44507</v>
       </c>
       <c r="E4" s="7">
         <f>IF(A4="","",SUMIF(J$16:J$30,'Release Plan'!A4,E$16:E$30))</f>
@@ -2291,8 +2264,8 @@
       <c r="G4" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="H4" s="10">
-        <v>44455</v>
+      <c r="H4" s="10" t="s">
+        <v>50</v>
       </c>
       <c r="I4" s="11" t="s">
         <v>41</v>
@@ -2462,14 +2435,14 @@
         <v>1</v>
       </c>
       <c r="B16" s="8">
-        <v>44448</v>
+        <v>44501</v>
       </c>
       <c r="C16" s="28">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D16" s="8">
         <f>IF(AND(B16&lt;&gt;"",C16&lt;&gt;""),B16+C16-1,"")</f>
-        <v>44455</v>
+        <v>44507</v>
       </c>
       <c r="E16" s="7">
         <v>5</v>
@@ -2481,7 +2454,7 @@
         <v>11</v>
       </c>
       <c r="H16" s="29">
-        <v>44455</v>
+        <v>44507</v>
       </c>
       <c r="I16" s="31" t="s">
         <v>17</v>
@@ -2499,14 +2472,14 @@
         <v>2</v>
       </c>
       <c r="B17" s="8">
-        <v>44456</v>
+        <v>44508</v>
       </c>
       <c r="C17" s="28">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D17" s="8">
         <f t="shared" ref="D17:D21" si="2">IF(AND(B17&lt;&gt;"",C17&lt;&gt;""),B17+C17-1,"")</f>
-        <v>44463</v>
+        <v>44514</v>
       </c>
       <c r="E17" s="7">
         <v>8</v>
@@ -2532,14 +2505,14 @@
         <v>3</v>
       </c>
       <c r="B18" s="8">
-        <v>44464</v>
+        <v>44515</v>
       </c>
       <c r="C18" s="28">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D18" s="8">
         <f t="shared" si="2"/>
-        <v>44471</v>
+        <v>44521</v>
       </c>
       <c r="E18" s="7">
         <v>8</v>
@@ -2565,14 +2538,14 @@
         <v>4</v>
       </c>
       <c r="B19" s="8">
-        <v>44472</v>
+        <v>44522</v>
       </c>
       <c r="C19" s="28">
         <v>6</v>
       </c>
       <c r="D19" s="8">
         <f t="shared" si="2"/>
-        <v>44477</v>
+        <v>44527</v>
       </c>
       <c r="E19" s="7">
         <v>6</v>
@@ -2598,14 +2571,14 @@
         <v>5</v>
       </c>
       <c r="B20" s="8">
-        <v>44478</v>
+        <v>44528</v>
       </c>
       <c r="C20" s="28">
         <v>7</v>
       </c>
       <c r="D20" s="8">
         <f t="shared" si="2"/>
-        <v>44484</v>
+        <v>44534</v>
       </c>
       <c r="E20" s="7">
         <v>7</v>
@@ -2631,7 +2604,7 @@
         <v>6</v>
       </c>
       <c r="B21" s="8" t="str">
-        <f t="shared" ref="B17:B30" si="4">IF(AND(B20&lt;&gt;"",C20&lt;&gt;"",C21&lt;&gt;""),B20+C20,"")</f>
+        <f t="shared" ref="B21:B30" si="4">IF(AND(B20&lt;&gt;"",C20&lt;&gt;"",C21&lt;&gt;""),B20+C20,"")</f>
         <v/>
       </c>
       <c r="C21" s="28"/>
@@ -2655,7 +2628,7 @@
       </c>
       <c r="C22" s="3"/>
       <c r="D22" s="32" t="str">
-        <f t="shared" ref="D16:D30" si="5">IF(AND(B22&lt;&gt;"",C22&lt;&gt;""),B22+C22-1,"")</f>
+        <f t="shared" ref="D22:D30" si="5">IF(AND(B22&lt;&gt;"",C22&lt;&gt;""),B22+C22-1,"")</f>
         <v/>
       </c>
       <c r="E22" s="15"/>
@@ -2916,53 +2889,53 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="H4:I10 E5:F10 E31:F32 A4:D10">
-    <cfRule type="expression" dxfId="40" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="36" priority="7" stopIfTrue="1">
       <formula>$G4="Planned"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="39" priority="8" stopIfTrue="1">
+    <cfRule type="expression" dxfId="35" priority="8" stopIfTrue="1">
       <formula>$G4="Ongoing"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G4:G10 G16:G30">
-    <cfRule type="expression" dxfId="38" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="34" priority="9" stopIfTrue="1">
       <formula>$G4="Planned"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="37" priority="10" stopIfTrue="1">
+    <cfRule type="expression" dxfId="33" priority="10" stopIfTrue="1">
       <formula>$G4="Ongoing"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="36" priority="11" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="11" stopIfTrue="1" operator="equal">
       <formula>"Unplanned"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E4:F5 F6 H16:I30 A16:F30">
-    <cfRule type="expression" dxfId="35" priority="12" stopIfTrue="1">
+    <cfRule type="expression" dxfId="31" priority="12" stopIfTrue="1">
       <formula>OR($G4="Planned",$G4="Unplanned")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="34" priority="13" stopIfTrue="1">
+    <cfRule type="expression" dxfId="30" priority="13" stopIfTrue="1">
       <formula>$G4="Ongoing"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B16:B21">
-    <cfRule type="expression" dxfId="33" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="29" priority="5" stopIfTrue="1">
       <formula>$G16="Planned"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="32" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="28" priority="6" stopIfTrue="1">
       <formula>$G16="Ongoing"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B16:B21">
-    <cfRule type="expression" dxfId="31" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="27" priority="3" stopIfTrue="1">
       <formula>$G16="Planned"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="30" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="26" priority="4" stopIfTrue="1">
       <formula>$G16="Ongoing"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D16:D21">
-    <cfRule type="expression" dxfId="29" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="25" priority="1" stopIfTrue="1">
       <formula>$G16="Planned"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="28" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="24" priority="2" stopIfTrue="1">
       <formula>$G16="Ongoing"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3776,90 +3749,90 @@
     <sortCondition ref="C5"/>
   </sortState>
   <conditionalFormatting sqref="H19:H27 A29:H138 B22:G27 A4:I4 H5:H12 I8:I12 A5:G13 B15:B19 H15:H16 A14:A27 C14:C21 D14:G19">
-    <cfRule type="expression" dxfId="27" priority="13" stopIfTrue="1">
+    <cfRule type="expression" dxfId="23" priority="13" stopIfTrue="1">
       <formula>$C4="Done"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="26" priority="14" stopIfTrue="1">
+    <cfRule type="expression" dxfId="22" priority="14" stopIfTrue="1">
       <formula>$C4="Ongoing"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="25" priority="15" stopIfTrue="1">
+    <cfRule type="expression" dxfId="21" priority="15" stopIfTrue="1">
       <formula>$C4="Removed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H28">
-    <cfRule type="expression" dxfId="24" priority="16" stopIfTrue="1">
+    <cfRule type="expression" dxfId="20" priority="16" stopIfTrue="1">
       <formula>$C18="Done"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="23" priority="17" stopIfTrue="1">
+    <cfRule type="expression" dxfId="19" priority="17" stopIfTrue="1">
       <formula>$C18="Ongoing"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="22" priority="18" stopIfTrue="1">
+    <cfRule type="expression" dxfId="18" priority="18" stopIfTrue="1">
       <formula>$C18="Removed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H17:H18">
-    <cfRule type="expression" dxfId="21" priority="19" stopIfTrue="1">
+    <cfRule type="expression" dxfId="17" priority="19" stopIfTrue="1">
       <formula>#REF!="Done"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="20" priority="20" stopIfTrue="1">
+    <cfRule type="expression" dxfId="16" priority="20" stopIfTrue="1">
       <formula>#REF!="Ongoing"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="19" priority="21" stopIfTrue="1">
+    <cfRule type="expression" dxfId="15" priority="21" stopIfTrue="1">
       <formula>#REF!="Removed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I6">
-    <cfRule type="expression" dxfId="18" priority="10" stopIfTrue="1">
+    <cfRule type="expression" dxfId="14" priority="10" stopIfTrue="1">
       <formula>$C6="Done"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="17" priority="11" stopIfTrue="1">
+    <cfRule type="expression" dxfId="13" priority="11" stopIfTrue="1">
       <formula>$C6="Ongoing"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="16" priority="12" stopIfTrue="1">
+    <cfRule type="expression" dxfId="12" priority="12" stopIfTrue="1">
       <formula>$C6="Removed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I5">
-    <cfRule type="expression" dxfId="15" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="11" priority="7" stopIfTrue="1">
       <formula>$C5="Done"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="14" priority="8" stopIfTrue="1">
+    <cfRule type="expression" dxfId="10" priority="8" stopIfTrue="1">
       <formula>$C5="Ongoing"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="13" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="9" priority="9" stopIfTrue="1">
       <formula>$C5="Removed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I7">
-    <cfRule type="expression" dxfId="12" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="8" priority="4" stopIfTrue="1">
       <formula>$C7="Done"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="11" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="7" priority="5" stopIfTrue="1">
       <formula>$C7="Ongoing"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="6" priority="6" stopIfTrue="1">
       <formula>$C7="Removed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H14:I14">
-    <cfRule type="expression" dxfId="9" priority="22" stopIfTrue="1">
+    <cfRule type="expression" dxfId="5" priority="22" stopIfTrue="1">
       <formula>$C13="Done"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="23" stopIfTrue="1">
+    <cfRule type="expression" dxfId="4" priority="23" stopIfTrue="1">
       <formula>$C13="Ongoing"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="7" priority="24" stopIfTrue="1">
+    <cfRule type="expression" dxfId="3" priority="24" stopIfTrue="1">
       <formula>$C13="Removed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H13:I13">
-    <cfRule type="expression" dxfId="6" priority="25" stopIfTrue="1">
+    <cfRule type="expression" dxfId="2" priority="25" stopIfTrue="1">
       <formula>#REF!="Done"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="5" priority="26" stopIfTrue="1">
+    <cfRule type="expression" dxfId="1" priority="26" stopIfTrue="1">
       <formula>#REF!="Ongoing"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="27" stopIfTrue="1">
+    <cfRule type="expression" dxfId="0" priority="27" stopIfTrue="1">
       <formula>#REF!="Removed"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>